<commit_message>
Updating files -> only minor corrections
</commit_message>
<xml_diff>
--- a/DLS_Plots/20231025_DLS_DMAPolymers_pDNA10_NP5_PBS01.xlsx
+++ b/DLS_Plots/20231025_DLS_DMAPolymers_pDNA10_NP5_PBS01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryellewright/Documents/Kumar-Biomaterials-Lab/DLS_Plots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C25A22-5083-7A48-A302-EFFE05AF0A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AB84F8-9A0D-CC49-B783-4028699F930A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5060" windowWidth="14020" windowHeight="11240" xr2:uid="{C36B8CCA-551F-D74A-A3C3-48AB2748738C}"/>
+    <workbookView xWindow="5980" yWindow="2980" windowWidth="14020" windowHeight="11240" xr2:uid="{C36B8CCA-551F-D74A-A3C3-48AB2748738C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <externalReferences>
     <externalReference r:id="rId2"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -516,7 +516,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>